<commit_message>
Cambio en el excel de carga
</commit_message>
<xml_diff>
--- a/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
+++ b/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
@@ -50,7 +50,7 @@
     <t>Número de factura</t>
   </si>
   <si>
-    <t>Fecha de compra</t>
+    <t>Fecha de compra (DD/MM/YYY)</t>
   </si>
   <si>
     <t>CATEGORÍAS</t>
@@ -148,15 +148,84 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -170,19 +239,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -195,28 +256,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,33 +278,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,43 +305,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -327,19 +327,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,109 +495,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,49 +507,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,32 +536,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,31 +560,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,23 +593,58 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -654,130 +654,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1320,8 +1320,8 @@
   <sheetPr/>
   <dimension ref="B1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -1335,8 +1335,8 @@
     <col min="8" max="8" width="13.8857142857143" style="4" customWidth="1"/>
     <col min="9" max="9" width="18.4380952380952" style="4" customWidth="1"/>
     <col min="10" max="10" width="15.4380952380952" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16.552380952381" style="4" customWidth="1"/>
-    <col min="12" max="12" width="15" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.5714285714286" style="4" customWidth="1"/>
+    <col min="12" max="12" width="28.5714285714286" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="76.2" customHeight="1" spans="2:3">

</xml_diff>

<commit_message>
Formato de fecha excel
</commit_message>
<xml_diff>
--- a/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
+++ b/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
@@ -147,11 +147,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -162,6 +163,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,8 +185,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -184,9 +208,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,49 +248,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -256,7 +271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,21 +293,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,187 +328,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,21 +546,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -590,6 +576,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -616,15 +626,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -636,7 +637,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -654,130 +655,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -788,16 +789,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1321,7 +1322,7 @@
   <dimension ref="B1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -1392,6 +1393,7 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" formatCells="0" objects="1"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Cambios excel de carga
</commit_message>
<xml_diff>
--- a/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
+++ b/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
@@ -11,14 +11,13 @@
     <sheet name="Categorías" sheetId="2" r:id="rId2"/>
     <sheet name="Estados" sheetId="3" r:id="rId3"/>
     <sheet name="Ubicaciones" sheetId="4" r:id="rId4"/>
-    <sheet name="Hoja5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Número de etiqueta</t>
   </si>
@@ -138,9 +137,6 @@
   </si>
   <si>
     <t>UBICACIONES</t>
-  </si>
-  <si>
-    <t>Edificio Principal</t>
   </si>
 </sst>
 </file>
@@ -148,8 +144,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy;@"/>
@@ -172,16 +168,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -193,8 +212,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,9 +236,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,7 +252,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -233,7 +260,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,13 +282,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -262,11 +289,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -276,36 +302,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -328,13 +324,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -346,169 +492,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,8 +535,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -561,6 +559,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -572,30 +579,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,20 +607,33 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -658,147 +654,171 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1319,81 +1339,104 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:L4"/>
+  <dimension ref="B1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="2" max="2" width="31.6666666666667" style="4" customWidth="1"/>
-    <col min="3" max="3" width="57.4380952380952" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.8857142857143" customWidth="1"/>
-    <col min="5" max="5" width="10.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="11.8857142857143" customWidth="1"/>
-    <col min="7" max="7" width="13.552380952381" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.8857142857143" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.4380952380952" style="4" customWidth="1"/>
-    <col min="10" max="10" width="15.4380952380952" style="5" customWidth="1"/>
-    <col min="11" max="11" width="17.5714285714286" style="4" customWidth="1"/>
-    <col min="12" max="12" width="28.5714285714286" style="6" customWidth="1"/>
+    <col min="2" max="2" width="31.6666666666667" style="7" customWidth="1"/>
+    <col min="3" max="3" width="57.4380952380952" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.8857142857143" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10.6666666666667" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.8857142857143" style="8" customWidth="1"/>
+    <col min="7" max="7" width="13.552380952381" style="7" customWidth="1"/>
+    <col min="8" max="8" width="13.8857142857143" style="7" customWidth="1"/>
+    <col min="9" max="9" width="18.4380952380952" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15.4380952380952" style="9" customWidth="1"/>
+    <col min="11" max="11" width="17.5714285714286" style="7" customWidth="1"/>
+    <col min="12" max="12" width="28.5714285714286" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="76.2" customHeight="1" spans="2:3">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="3" spans="2:12">
-      <c r="B3" s="8" t="s">
+    <row r="1" ht="76.2" customHeight="1" spans="2:12">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" s="4" customFormat="1" spans="2:12">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="13"/>
+    <row r="4" spans="2:14">
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="21"/>
+      <c r="N4" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" objects="1"/>
+  <sheetProtection sheet="1" formatCells="0" insertRows="0" objects="1"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
@@ -1420,24 +1463,24 @@
   <dimension ref="B1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="20.1047619047619" customWidth="1"/>
+    <col min="2" max="2" width="20.1047619047619" style="4" customWidth="1"/>
     <col min="3" max="3" width="83.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="69.6" customHeight="1"/>
     <row r="3" spans="2:3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1445,7 +1488,7 @@
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1453,7 +1496,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1461,23 +1504,23 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="2" t="s">
+    <row r="8" s="4" customFormat="1" spans="2:3">
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1485,7 +1528,7 @@
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1509,7 +1552,7 @@
   <dimension ref="B1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1588,7 +1631,7 @@
   <dimension ref="B1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B2" sqref="B$1:B$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1604,9 +1647,7 @@
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1616,20 +1657,4 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios Plantilla  Excel y Cambios de Toma Fisica
</commit_message>
<xml_diff>
--- a/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
+++ b/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7965"/>
+    <workbookView windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de activos" sheetId="1" r:id="rId1"/>
-    <sheet name="Categorías" sheetId="2" r:id="rId2"/>
-    <sheet name="Estados" sheetId="3" r:id="rId3"/>
-    <sheet name="Ubicaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="Categorías" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Estados" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="Ubicaciones" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Número de etiqueta</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Terrenos</t>
   </si>
   <si>
-    <t>Aquellos terrenos que posea la empresa, donde se encuentren o no la fábrica, oficina, bodega, etc.</t>
+    <t>Aquellos terrenos que posea la empresa, donde se encuentren o no la fábrica, oficina, bodega, etc.</t>
   </si>
   <si>
     <t>Construcciones</t>
@@ -91,6 +91,12 @@
     <t>Medios de transporte de la compañía, como coches, camiones, motos, barcos, aviones, etc.</t>
   </si>
   <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aplicativos de Software no Tangibles </t>
+  </si>
+  <si>
     <t>Otros</t>
   </si>
   <si>
@@ -115,7 +121,7 @@
     <t>Sin uso</t>
   </si>
   <si>
-    <t>Activo fijo que está en buen estado pero no se encuentra en uso, almacenado en una bodega o estante.</t>
+    <t>Activo fijo que está en buen estado pero no se encuentra en uso, almacenado en bodega o estante.</t>
   </si>
   <si>
     <t>Dañado</t>
@@ -137,20 +143,41 @@
   </si>
   <si>
     <t>UBICACIONES</t>
+  </si>
+  <si>
+    <t>725</t>
+  </si>
+  <si>
+    <t>Ubicacion Alfa</t>
+  </si>
+  <si>
+    <t>Ubicacion 2</t>
+  </si>
+  <si>
+    <t>Ubicacion 3</t>
+  </si>
+  <si>
+    <t>Ubicacion 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubicacion 6 </t>
+  </si>
+  <si>
+    <t>Ubicacion 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,28 +190,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -192,7 +198,92 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -200,76 +291,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -277,29 +298,28 @@
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -324,61 +344,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,121 +524,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,22 +553,50 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -564,15 +612,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,197 +634,177 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -802,7 +821,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -811,8 +831,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -822,52 +844,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1339,67 +1361,67 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:N4"/>
+  <dimension ref="B1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="2" max="2" width="31.6666666666667" style="7" customWidth="1"/>
-    <col min="3" max="3" width="57.4380952380952" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.8857142857143" style="8" customWidth="1"/>
-    <col min="5" max="5" width="10.6666666666667" style="8" customWidth="1"/>
-    <col min="6" max="6" width="11.8857142857143" style="8" customWidth="1"/>
-    <col min="7" max="7" width="13.552380952381" style="7" customWidth="1"/>
-    <col min="8" max="8" width="13.8857142857143" style="7" customWidth="1"/>
-    <col min="9" max="9" width="18.4380952380952" style="7" customWidth="1"/>
-    <col min="10" max="10" width="15.4380952380952" style="9" customWidth="1"/>
-    <col min="11" max="11" width="17.5714285714286" style="7" customWidth="1"/>
-    <col min="12" max="12" width="28.5714285714286" style="10" customWidth="1"/>
+    <col min="2" max="2" width="31.6666666666667" style="6" customWidth="1"/>
+    <col min="3" max="3" width="57.4380952380952" style="6" customWidth="1"/>
+    <col min="4" max="4" width="12.8857142857143" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.6666666666667" style="7" customWidth="1"/>
+    <col min="6" max="6" width="11.8857142857143" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.552380952381" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.8857142857143" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.4380952380952" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.4380952380952" style="8" customWidth="1"/>
+    <col min="11" max="11" width="17.5714285714286" style="6" customWidth="1"/>
+    <col min="12" max="12" width="28.5714285714286" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="76.2" customHeight="1" spans="2:12">
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+    <row r="1" s="5" customFormat="1" ht="76.2" customHeight="1" spans="2:12">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
       <c r="J1" s="16"/>
-      <c r="K1" s="12"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="17"/>
     </row>
     <row r="2" spans="2:12">
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
-      <c r="J2" s="16"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="12"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" s="4" customFormat="1" spans="2:12">
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" customFormat="1" spans="2:12">
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="13" t="s">
@@ -1411,17 +1433,17 @@
       <c r="I3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="20" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:12">
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -1430,25 +1452,24 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
-      <c r="J4" s="20"/>
+      <c r="J4" s="22"/>
       <c r="K4" s="14"/>
-      <c r="L4" s="21"/>
-      <c r="N4" s="4"/>
+      <c r="L4" s="23"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" insertRows="0" objects="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteColumns="0" deleteRows="0" objects="1"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
-      <formula1>Categorías!$B$4:$B$10</formula1>
+      <formula1>Categorías!$B$4:$B$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E$1:E$1048576">
+      <formula1>Estados!$B$4:$B$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F$1:F$1048576">
       <formula1>Ubicaciones!$B$4:$B$52</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E$1:E$1048576">
-      <formula1>Estados!$B$4:$B$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1460,27 +1481,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="20.1047619047619" style="4" customWidth="1"/>
-    <col min="3" max="3" width="83.8857142857143" customWidth="1"/>
+    <col min="2" max="2" width="20.1047619047619" customWidth="1"/>
+    <col min="3" max="3" width="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="69.6" customHeight="1"/>
     <row r="3" spans="2:3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1488,7 +1509,7 @@
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1496,7 +1517,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1504,23 +1525,23 @@
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" s="4" customFormat="1" spans="2:3">
-      <c r="B8" s="6" t="s">
+    <row r="8" customFormat="1" spans="2:3">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:3">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1528,15 +1549,23 @@
       </c>
     </row>
     <row r="10" spans="2:3">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
@@ -1553,7 +1582,7 @@
   <dimension ref="B1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1564,60 +1593,60 @@
     <row r="1" ht="63.6" customHeight="1"/>
     <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:3">
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
@@ -1630,13 +1659,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:C4"/>
+  <dimension ref="B1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="57.8857142857143" customWidth="1"/>
   </cols>
@@ -1645,14 +1674,46 @@
     <row r="2" ht="14.4" customHeight="1"/>
     <row r="3" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Alinear textos en seleccion del plan (falta btn mensual)
</commit_message>
<xml_diff>
--- a/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
+++ b/ActiveSmartWeb/PlantillaExcelReporte/ExcelcargaSIGNUSID.xlsx
@@ -170,12 +170,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.0;\-&quot;$&quot;#,##0.0"/>
+    <numFmt numFmtId="180" formatCode="&quot;$&quot;#,###.##000_);[Red]\(&quot;$&quot;#,###.##000\)"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -798,12 +800,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
@@ -833,9 +834,9 @@
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
@@ -1361,58 +1362,55 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:L4"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="11.4380952380952" defaultRowHeight="15" outlineLevelRow="6"/>
   <cols>
-    <col min="2" max="2" width="31.6666666666667" style="6" customWidth="1"/>
-    <col min="3" max="3" width="57.4380952380952" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.8857142857143" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.6666666666667" style="7" customWidth="1"/>
-    <col min="6" max="6" width="11.8857142857143" style="7" customWidth="1"/>
-    <col min="7" max="7" width="13.552380952381" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.8857142857143" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.4380952380952" style="6" customWidth="1"/>
-    <col min="10" max="10" width="15.4380952380952" style="8" customWidth="1"/>
-    <col min="11" max="11" width="17.5714285714286" style="6" customWidth="1"/>
-    <col min="12" max="12" width="28.5714285714286" style="9" customWidth="1"/>
+    <col min="2" max="2" width="31.6666666666667" style="5" customWidth="1"/>
+    <col min="3" max="3" width="57.4380952380952" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12.8857142857143" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.6666666666667" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.8857142857143" style="6" customWidth="1"/>
+    <col min="7" max="7" width="13.552380952381" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.8857142857143" style="5" customWidth="1"/>
+    <col min="9" max="9" width="18.4380952380952" style="5" customWidth="1"/>
+    <col min="10" max="10" width="31.8571428571429" style="7" customWidth="1"/>
+    <col min="11" max="11" width="17.5714285714286" style="5" customWidth="1"/>
+    <col min="12" max="12" width="28.5714285714286" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="76.2" customHeight="1" spans="2:12">
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="17"/>
+    <row r="1" s="4" customFormat="1" ht="76.2" customHeight="1" spans="2:12">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="19"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" customFormat="1" spans="2:12">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1424,37 +1422,54 @@
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="21">
+        <v>5453535345.65756</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="22"/>
+    </row>
+    <row r="5" spans="10:10">
+      <c r="J5" s="7">
+        <v>3.45343453434345e+18</v>
+      </c>
+    </row>
+    <row r="6" spans="10:10">
+      <c r="J6" s="7">
+        <v>4.35345345345345e+21</v>
+      </c>
+    </row>
+    <row r="7" spans="10:10">
+      <c r="J7" s="7">
+        <v>34543543.345434</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteColumns="0" deleteRows="0" objects="1"/>
@@ -1557,10 +1572,10 @@
       </c>
     </row>
     <row r="11" spans="2:3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>